<commit_message>
Sync apostille order form and backend changes
</commit_message>
<xml_diff>
--- a/order-form/Spread Sheets & Scripts/Shipping-Options-Pricing.xlsx
+++ b/order-form/Spread Sheets & Scripts/Shipping-Options-Pricing.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t xml:space="preserve">Carrier</t>
   </si>
@@ -75,15 +75,18 @@
     <t xml:space="preserve">time_window</t>
   </si>
   <si>
+    <t xml:space="preserve">Priority</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">usps_domestic_priority</t>
+  </si>
+  <si>
     <t xml:space="preserve">Priority Express</t>
   </si>
   <si>
-    <t xml:space="preserve">2-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">usps_domestic_priority</t>
-  </si>
-  <si>
     <t xml:space="preserve">1-2</t>
   </si>
   <si>
@@ -108,7 +111,7 @@
     <t xml:space="preserve">fedex_domestic_2day</t>
   </si>
   <si>
-    <t xml:space="preserve">Overnight</t>
+    <t xml:space="preserve">Overnight 8 PM</t>
   </si>
   <si>
     <t xml:space="preserve">1</t>
@@ -117,7 +120,13 @@
     <t xml:space="preserve">fedex_domestic_overnight_8pm</t>
   </si>
   <si>
+    <t xml:space="preserve">Overnight 12 PM</t>
+  </si>
+  <si>
     <t xml:space="preserve">fedex_domestic_overnight_12am</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Overnight 8 AM</t>
   </si>
   <si>
     <t xml:space="preserve">fedex_domestic_first_8am</t>
@@ -561,7 +570,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="B33" activeCellId="0" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -615,16 +624,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E3" s="3" t="n">
         <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -632,16 +641,16 @@
         <v>5</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E4" s="3" t="n">
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -649,16 +658,16 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E5" s="3" t="n">
         <v>45</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -666,19 +675,19 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" s="4" t="n">
         <v>0.833333333333333</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E6" s="3" t="n">
         <v>65</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -686,19 +695,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="C7" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E7" s="3" t="n">
         <v>70</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -706,19 +715,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C8" s="4" t="n">
         <v>0.333333333333333</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E8" s="3" t="n">
         <v>120</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -770,10 +779,10 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="C2" s="3" t="n">
         <v>0</v>
@@ -782,15 +791,15 @@
         <v>65</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="C3" s="3" t="n">
         <v>0</v>
@@ -799,15 +808,15 @@
         <v>130</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="n">
         <v>0</v>
@@ -816,7 +825,7 @@
         <v>130</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>